<commit_message>
380 test over testrs
</commit_message>
<xml_diff>
--- a/0咪咕音乐/咪咕音乐v380/咪咕音乐Jadeite_USS_music-V3.8.0版本用例.xlsx
+++ b/0咪咕音乐/咪咕音乐v380/咪咕音乐Jadeite_USS_music-V3.8.0版本用例.xlsx
@@ -10,14 +10,14 @@
     <sheet name="后台流程类" sheetId="6" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">后台流程类!$A$1:$AB$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">后台流程类!$A$1:$AB$68</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="177">
   <si>
     <t>*功能模块</t>
   </si>
@@ -301,6 +301,18 @@
     <t>1、返回报文中无知识付费音频</t>
   </si>
   <si>
+    <t>知识付费专辑和在售专辑不同时显示</t>
+  </si>
+  <si>
+    <t>1、数据可设置知识付费专辑和在售同时存在
+2、接口请求目标专辑
+3、产看返回报文</t>
+  </si>
+  <si>
+    <t>1、接口请求成功
+2、返回报文中ispay=1，isinsaledata=0</t>
+  </si>
+  <si>
     <t>versionNo大于3.6.0搜索付费专辑</t>
   </si>
   <si>
@@ -606,7 +618,7 @@
   </si>
   <si>
     <t>1、返回键入搜索词相关结果
-2、现网DX纠错为当然，dx纠错为稻香。应该都是稻香</t>
+2、现网DX纠错为当然，dx纠错为稻香。应该一致</t>
   </si>
   <si>
     <t>39、Flavor Of Life （Flavor Of Life 联想提示优化</t>
@@ -637,8 +649,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -704,8 +716,53 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -726,56 +783,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -785,18 +792,17 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -809,18 +815,17 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -842,7 +847,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -869,7 +881,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -881,7 +941,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -893,13 +983,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -911,19 +1013,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -935,121 +1055,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1165,11 +1177,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1191,11 +1209,27 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1211,15 +1245,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1241,24 +1266,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1270,10 +1282,10 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1282,137 +1294,137 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1478,6 +1490,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1870,12 +1888,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AB71"/>
+  <dimension ref="A1:AB72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="L57" sqref="L57"/>
+      <selection pane="bottomLeft" activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15"/>
@@ -1960,9 +1978,9 @@
       <c r="T1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
     </row>
     <row r="2" ht="24" spans="1:24">
       <c r="A2" s="10" t="s">
@@ -1987,10 +2005,10 @@
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
       <c r="T2" s="10"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="60" spans="1:20">
       <c r="A3" s="10"/>
@@ -2057,23 +2075,23 @@
         <v>25</v>
       </c>
       <c r="J5" s="16"/>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="30" t="s">
         <v>26</v>
       </c>
       <c r="L5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="29"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="36"/>
+      <c r="S5" s="36"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A6" s="17"/>
@@ -2092,23 +2110,23 @@
         <v>25</v>
       </c>
       <c r="J6" s="16"/>
-      <c r="K6" s="28" t="s">
+      <c r="K6" s="30" t="s">
         <v>31</v>
       </c>
       <c r="L6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N6" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O6" s="19"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A7" s="17"/>
@@ -2127,23 +2145,23 @@
         <v>25</v>
       </c>
       <c r="J7" s="12"/>
-      <c r="K7" s="28" t="s">
+      <c r="K7" s="30" t="s">
         <v>26</v>
       </c>
       <c r="L7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="28" t="s">
+      <c r="M7" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N7" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O7" s="19"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="35"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A8" s="17"/>
@@ -2162,23 +2180,23 @@
         <v>25</v>
       </c>
       <c r="J8" s="12"/>
-      <c r="K8" s="28" t="s">
+      <c r="K8" s="30" t="s">
         <v>31</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M8" s="28" t="s">
+      <c r="M8" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N8" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O8" s="19"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="35"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="60" spans="1:19">
       <c r="A9" s="11"/>
@@ -2197,23 +2215,23 @@
         <v>25</v>
       </c>
       <c r="J9" s="16"/>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L9" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="28" t="s">
+      <c r="M9" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="29"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="36"/>
+      <c r="S9" s="36"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="60" spans="1:19">
       <c r="A10" s="11"/>
@@ -2232,23 +2250,23 @@
         <v>25</v>
       </c>
       <c r="J10" s="16"/>
-      <c r="K10" s="28" t="s">
+      <c r="K10" s="30" t="s">
         <v>42</v>
       </c>
       <c r="L10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="M10" s="28" t="s">
+      <c r="M10" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N10" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="35"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
     </row>
     <row r="11" s="1" customFormat="1" ht="60" spans="1:19">
       <c r="A11" s="11"/>
@@ -2267,23 +2285,23 @@
         <v>25</v>
       </c>
       <c r="J11" s="16"/>
-      <c r="K11" s="28" t="s">
+      <c r="K11" s="30" t="s">
         <v>44</v>
       </c>
       <c r="L11" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="M11" s="28" t="s">
+      <c r="M11" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="35"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
     </row>
     <row r="12" s="1" customFormat="1" ht="60" spans="1:19">
       <c r="A12" s="11"/>
@@ -2302,23 +2320,23 @@
         <v>25</v>
       </c>
       <c r="J12" s="16"/>
-      <c r="K12" s="28" t="s">
+      <c r="K12" s="30" t="s">
         <v>47</v>
       </c>
       <c r="L12" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="M12" s="28" t="s">
+      <c r="M12" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N12" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
     </row>
     <row r="13" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A13" s="11"/>
@@ -2337,23 +2355,23 @@
         <v>25</v>
       </c>
       <c r="J13" s="16"/>
-      <c r="K13" s="28" t="s">
+      <c r="K13" s="30" t="s">
         <v>49</v>
       </c>
       <c r="L13" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="M13" s="28" t="s">
+      <c r="M13" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N13" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
     </row>
     <row r="14" s="1" customFormat="1" ht="24" spans="1:20">
       <c r="A14" s="10"/>
@@ -2402,17 +2420,17 @@
       <c r="L15" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="M15" s="28" t="s">
+      <c r="M15" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N15" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O15" s="19"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="29"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="37"/>
     </row>
     <row r="16" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A16" s="19"/>
@@ -2437,17 +2455,17 @@
       <c r="L16" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="M16" s="28" t="s">
+      <c r="M16" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N16" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O16" s="19"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
     </row>
     <row r="17" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A17" s="19"/>
@@ -2472,17 +2490,17 @@
       <c r="L17" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="M17" s="28" t="s">
+      <c r="M17" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N17" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O17" s="19"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="37"/>
     </row>
     <row r="18" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A18" s="19"/>
@@ -2507,17 +2525,17 @@
       <c r="L18" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="M18" s="28" t="s">
+      <c r="M18" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N18" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O18" s="19"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="37"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="30" spans="1:19">
       <c r="A19" s="19"/>
@@ -2542,17 +2560,17 @@
       <c r="L19" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="M19" s="28" t="s">
+      <c r="M19" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N19" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O19" s="19"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29"/>
-      <c r="R19" s="35"/>
-      <c r="S19" s="35"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="37"/>
+      <c r="S19" s="37"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="30" spans="1:19">
       <c r="A20" s="19"/>
@@ -2577,17 +2595,17 @@
       <c r="L20" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="M20" s="28" t="s">
+      <c r="M20" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N20" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O20" s="19"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="35"/>
-      <c r="S20" s="35"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="30" spans="1:19">
       <c r="A21" s="19"/>
@@ -2612,17 +2630,17 @@
       <c r="L21" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="M21" s="28" t="s">
+      <c r="M21" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N21" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O21" s="19"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="35"/>
-      <c r="S21" s="35"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="37"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="30" spans="1:19">
       <c r="A22" s="19"/>
@@ -2647,17 +2665,17 @@
       <c r="L22" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="M22" s="28" t="s">
+      <c r="M22" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N22" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O22" s="19"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="35"/>
-      <c r="S22" s="35"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="30" spans="1:19">
       <c r="A23" s="19"/>
@@ -2682,17 +2700,17 @@
       <c r="L23" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="M23" s="28" t="s">
+      <c r="M23" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N23" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O23" s="19"/>
-      <c r="P23" s="29"/>
-      <c r="Q23" s="29"/>
-      <c r="R23" s="35"/>
-      <c r="S23" s="35"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="37"/>
+      <c r="S23" s="37"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="30" spans="1:19">
       <c r="A24" s="19"/>
@@ -2717,17 +2735,17 @@
       <c r="L24" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="M24" s="28" t="s">
+      <c r="M24" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N24" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O24" s="19"/>
-      <c r="P24" s="29"/>
-      <c r="Q24" s="29"/>
-      <c r="R24" s="35"/>
-      <c r="S24" s="35"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="37"/>
     </row>
     <row r="25" s="1" customFormat="1" ht="30" spans="1:19">
       <c r="A25" s="19"/>
@@ -2752,17 +2770,17 @@
       <c r="L25" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="M25" s="28" t="s">
+      <c r="M25" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N25" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O25" s="19"/>
-      <c r="P25" s="29"/>
-      <c r="Q25" s="29"/>
-      <c r="R25" s="35"/>
-      <c r="S25" s="35"/>
+      <c r="P25" s="31"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
     </row>
     <row r="26" s="1" customFormat="1" ht="30" spans="1:19">
       <c r="A26" s="19"/>
@@ -2787,22 +2805,22 @@
       <c r="L26" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="M26" s="28" t="s">
+      <c r="M26" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N26" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O26" s="19"/>
-      <c r="P26" s="29"/>
-      <c r="Q26" s="29"/>
-      <c r="R26" s="35"/>
-      <c r="S26" s="35"/>
-    </row>
-    <row r="27" s="1" customFormat="1" ht="30" spans="1:19">
+      <c r="P26" s="31"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="37"/>
+      <c r="S26" s="37"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="60" spans="1:19">
       <c r="A27" s="19"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="21"/>
       <c r="E27" s="11"/>
       <c r="F27" s="21" t="s">
@@ -2822,17 +2840,17 @@
       <c r="L27" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="M27" s="28" t="s">
+      <c r="M27" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N27" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O27" s="19"/>
-      <c r="P27" s="29"/>
-      <c r="Q27" s="29"/>
-      <c r="R27" s="35"/>
-      <c r="S27" s="35"/>
+      <c r="P27" s="31"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37"/>
     </row>
     <row r="28" s="1" customFormat="1" ht="30" spans="1:19">
       <c r="A28" s="19"/>
@@ -2845,29 +2863,29 @@
       </c>
       <c r="G28" s="11"/>
       <c r="H28" s="16" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I28" s="15" t="s">
         <v>53</v>
       </c>
       <c r="J28" s="12"/>
       <c r="K28" s="11" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="M28" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="M28" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N28" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O28" s="19"/>
-      <c r="P28" s="29"/>
-      <c r="Q28" s="29"/>
-      <c r="R28" s="35"/>
-      <c r="S28" s="35"/>
+      <c r="P28" s="31"/>
+      <c r="Q28" s="31"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37"/>
     </row>
     <row r="29" s="1" customFormat="1" ht="30" spans="1:19">
       <c r="A29" s="19"/>
@@ -2876,7 +2894,7 @@
       <c r="D29" s="21"/>
       <c r="E29" s="11"/>
       <c r="F29" s="21" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G29" s="11"/>
       <c r="H29" s="16" t="s">
@@ -2887,97 +2905,97 @@
       </c>
       <c r="J29" s="12"/>
       <c r="K29" s="11" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="L29" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="M29" s="28" t="s">
+      <c r="M29" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N29" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O29" s="19"/>
-      <c r="P29" s="29"/>
-      <c r="Q29" s="29"/>
-      <c r="R29" s="35"/>
-      <c r="S29" s="35"/>
-    </row>
-    <row r="30" s="1" customFormat="1" ht="14.4" spans="1:20">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
-      <c r="T30" s="10"/>
-    </row>
-    <row r="31" s="1" customFormat="1" ht="30" spans="1:19">
-      <c r="A31" s="19"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="21" t="s">
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="37"/>
+      <c r="S29" s="37"/>
+    </row>
+    <row r="30" s="1" customFormat="1" ht="30" spans="1:19">
+      <c r="A30" s="19"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="G31" s="11"/>
-      <c r="H31" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I31" s="15" t="s">
+      <c r="G30" s="11"/>
+      <c r="H30" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="J30" s="12"/>
+      <c r="K30" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="L30" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="J31" s="12"/>
-      <c r="K31" s="11" t="s">
+      <c r="M30" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N30" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="O30" s="19"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="37"/>
+      <c r="S30" s="37"/>
+    </row>
+    <row r="31" s="1" customFormat="1" ht="14.4" spans="1:20">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="L31" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="M31" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N31" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="O31" s="19"/>
-      <c r="P31" s="29"/>
-      <c r="Q31" s="29"/>
-      <c r="R31" s="35"/>
-      <c r="S31" s="35"/>
-    </row>
-    <row r="32" s="1" customFormat="1" ht="45" spans="1:19">
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+    </row>
+    <row r="32" s="1" customFormat="1" ht="30" spans="1:19">
       <c r="A32" s="19"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
       <c r="D32" s="21"/>
       <c r="E32" s="11"/>
       <c r="F32" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G32" s="11"/>
       <c r="H32" s="16" t="s">
         <v>24</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="11" t="s">
@@ -2986,48 +3004,59 @@
       <c r="L32" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="M32" s="28" t="s">
+      <c r="M32" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N32" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O32" s="19"/>
-      <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
-      <c r="R32" s="35"/>
-      <c r="S32" s="35"/>
-    </row>
-    <row r="33" s="1" customFormat="1" ht="48" spans="1:20">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10" t="s">
+      <c r="P32" s="31"/>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="37"/>
+    </row>
+    <row r="33" s="1" customFormat="1" ht="45" spans="1:19">
+      <c r="A33" s="19"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="10"/>
-      <c r="T33" s="10"/>
-    </row>
-    <row r="34" s="1" customFormat="1" ht="14.4" spans="1:20">
+      <c r="G33" s="11"/>
+      <c r="H33" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="J33" s="12"/>
+      <c r="K33" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="L33" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="M33" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N33" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="O33" s="19"/>
+      <c r="P33" s="31"/>
+      <c r="Q33" s="31"/>
+      <c r="R33" s="37"/>
+      <c r="S33" s="37"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="48" spans="1:20">
       <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="B34" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -3046,40 +3075,29 @@
       <c r="S34" s="10"/>
       <c r="T34" s="10"/>
     </row>
-    <row r="35" s="1" customFormat="1" ht="45" spans="1:19">
-      <c r="A35" s="19"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="G35" s="11"/>
-      <c r="H35" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J35" s="12"/>
-      <c r="K35" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="L35" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="M35" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N35" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="O35" s="19"/>
-      <c r="P35" s="29"/>
-      <c r="Q35" s="29"/>
-      <c r="R35" s="35"/>
-      <c r="S35" s="35"/>
+    <row r="35" s="1" customFormat="1" ht="14.4" spans="1:20">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
     </row>
     <row r="36" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A36" s="19"/>
@@ -3092,32 +3110,32 @@
       </c>
       <c r="G36" s="11"/>
       <c r="H36" s="16" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I36" s="15" t="s">
         <v>25</v>
       </c>
       <c r="J36" s="12"/>
-      <c r="K36" s="28" t="s">
+      <c r="K36" s="30" t="s">
         <v>100</v>
       </c>
       <c r="L36" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="M36" s="28" t="s">
+      <c r="M36" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N36" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O36" s="19"/>
-      <c r="P36" s="29"/>
-      <c r="Q36" s="29"/>
-      <c r="R36" s="35"/>
-      <c r="S36" s="35"/>
+      <c r="P36" s="31"/>
+      <c r="Q36" s="31"/>
+      <c r="R36" s="37"/>
+      <c r="S36" s="37"/>
     </row>
     <row r="37" s="1" customFormat="1" ht="45" spans="1:19">
-      <c r="A37" s="21"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
       <c r="D37" s="21"/>
@@ -3127,29 +3145,29 @@
       </c>
       <c r="G37" s="11"/>
       <c r="H37" s="16" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="I37" s="15" t="s">
         <v>25</v>
       </c>
       <c r="J37" s="12"/>
-      <c r="K37" s="28" t="s">
+      <c r="K37" s="30" t="s">
         <v>103</v>
       </c>
       <c r="L37" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="M37" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="M37" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N37" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O37" s="19"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="29"/>
-      <c r="R37" s="35"/>
-      <c r="S37" s="35"/>
+      <c r="P37" s="31"/>
+      <c r="Q37" s="31"/>
+      <c r="R37" s="37"/>
+      <c r="S37" s="37"/>
     </row>
     <row r="38" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A38" s="21"/>
@@ -3158,33 +3176,33 @@
       <c r="D38" s="21"/>
       <c r="E38" s="11"/>
       <c r="F38" s="21" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G38" s="11"/>
       <c r="H38" s="16" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I38" s="15" t="s">
         <v>25</v>
       </c>
       <c r="J38" s="12"/>
-      <c r="K38" s="28" t="s">
-        <v>105</v>
+      <c r="K38" s="30" t="s">
+        <v>106</v>
       </c>
       <c r="L38" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="M38" s="28" t="s">
+      <c r="M38" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N38" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O38" s="19"/>
-      <c r="P38" s="29"/>
-      <c r="Q38" s="29"/>
-      <c r="R38" s="35"/>
-      <c r="S38" s="35"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="31"/>
+      <c r="R38" s="37"/>
+      <c r="S38" s="37"/>
     </row>
     <row r="39" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A39" s="21"/>
@@ -3193,7 +3211,7 @@
       <c r="D39" s="21"/>
       <c r="E39" s="11"/>
       <c r="F39" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G39" s="11"/>
       <c r="H39" s="16" t="s">
@@ -3203,23 +3221,23 @@
         <v>25</v>
       </c>
       <c r="J39" s="12"/>
-      <c r="K39" s="28" t="s">
-        <v>107</v>
+      <c r="K39" s="30" t="s">
+        <v>108</v>
       </c>
       <c r="L39" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="M39" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="M39" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N39" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O39" s="19"/>
-      <c r="P39" s="29"/>
-      <c r="Q39" s="29"/>
-      <c r="R39" s="35"/>
-      <c r="S39" s="35"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="31"/>
+      <c r="R39" s="37"/>
+      <c r="S39" s="37"/>
     </row>
     <row r="40" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A40" s="21"/>
@@ -3228,7 +3246,7 @@
       <c r="D40" s="21"/>
       <c r="E40" s="11"/>
       <c r="F40" s="21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G40" s="11"/>
       <c r="H40" s="16" t="s">
@@ -3238,23 +3256,23 @@
         <v>25</v>
       </c>
       <c r="J40" s="12"/>
-      <c r="K40" s="28" t="s">
-        <v>109</v>
+      <c r="K40" s="30" t="s">
+        <v>110</v>
       </c>
       <c r="L40" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="M40" s="28" t="s">
+      <c r="M40" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N40" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O40" s="19"/>
-      <c r="P40" s="29"/>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="35"/>
-      <c r="S40" s="35"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="31"/>
+      <c r="R40" s="37"/>
+      <c r="S40" s="37"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A41" s="21"/>
@@ -3263,7 +3281,7 @@
       <c r="D41" s="21"/>
       <c r="E41" s="11"/>
       <c r="F41" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G41" s="11"/>
       <c r="H41" s="16" t="s">
@@ -3273,23 +3291,23 @@
         <v>25</v>
       </c>
       <c r="J41" s="12"/>
-      <c r="K41" s="28" t="s">
-        <v>97</v>
+      <c r="K41" s="30" t="s">
+        <v>112</v>
       </c>
       <c r="L41" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="M41" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="M41" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N41" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O41" s="19"/>
-      <c r="P41" s="29"/>
-      <c r="Q41" s="29"/>
-      <c r="R41" s="35"/>
-      <c r="S41" s="35"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="37"/>
+      <c r="S41" s="37"/>
     </row>
     <row r="42" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A42" s="21"/>
@@ -3298,7 +3316,7 @@
       <c r="D42" s="21"/>
       <c r="E42" s="11"/>
       <c r="F42" s="21" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G42" s="11"/>
       <c r="H42" s="16" t="s">
@@ -3308,82 +3326,82 @@
         <v>25</v>
       </c>
       <c r="J42" s="12"/>
-      <c r="K42" s="28" t="s">
+      <c r="K42" s="30" t="s">
         <v>100</v>
       </c>
       <c r="L42" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="M42" s="28" t="s">
+      <c r="M42" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N42" s="15" t="s">
         <v>29</v>
       </c>
       <c r="O42" s="19"/>
-      <c r="P42" s="29"/>
-      <c r="Q42" s="29"/>
-      <c r="R42" s="35"/>
-      <c r="S42" s="35"/>
-    </row>
-    <row r="43" s="1" customFormat="1" ht="14.4" spans="1:20">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-      <c r="S43" s="10"/>
-      <c r="T43" s="10"/>
-    </row>
-    <row r="44" s="1" customFormat="1" ht="45" spans="1:19">
-      <c r="A44" s="21"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="G44" s="11"/>
-      <c r="H44" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I44" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="J44" s="12"/>
-      <c r="K44" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="L44" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="M44" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N44" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="O44" s="29"/>
-      <c r="P44" s="29"/>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="35"/>
-      <c r="S44" s="35"/>
+      <c r="P42" s="31"/>
+      <c r="Q42" s="31"/>
+      <c r="R42" s="37"/>
+      <c r="S42" s="37"/>
+    </row>
+    <row r="43" s="1" customFormat="1" ht="45" spans="1:19">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="G43" s="11"/>
+      <c r="H43" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J43" s="12"/>
+      <c r="K43" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="L43" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="M43" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N43" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="O43" s="19"/>
+      <c r="P43" s="31"/>
+      <c r="Q43" s="31"/>
+      <c r="R43" s="37"/>
+      <c r="S43" s="37"/>
+    </row>
+    <row r="44" s="1" customFormat="1" ht="14.4" spans="1:20">
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="10"/>
+      <c r="S44" s="10"/>
+      <c r="T44" s="10"/>
     </row>
     <row r="45" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A45" s="21"/>
@@ -3392,33 +3410,33 @@
       <c r="D45" s="21"/>
       <c r="E45" s="11"/>
       <c r="F45" s="21" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="16" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I45" s="15" t="s">
         <v>53</v>
       </c>
       <c r="J45" s="12"/>
-      <c r="K45" s="28" t="s">
+      <c r="K45" s="30" t="s">
         <v>100</v>
       </c>
       <c r="L45" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="M45" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="M45" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N45" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O45" s="29"/>
-      <c r="P45" s="29"/>
-      <c r="Q45" s="29"/>
-      <c r="R45" s="35"/>
-      <c r="S45" s="35"/>
+      <c r="O45" s="31"/>
+      <c r="P45" s="31"/>
+      <c r="Q45" s="31"/>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
     </row>
     <row r="46" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A46" s="21"/>
@@ -3427,7 +3445,7 @@
       <c r="D46" s="21"/>
       <c r="E46" s="11"/>
       <c r="F46" s="21" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G46" s="11"/>
       <c r="H46" s="16" t="s">
@@ -3437,23 +3455,23 @@
         <v>53</v>
       </c>
       <c r="J46" s="12"/>
-      <c r="K46" s="28" t="s">
-        <v>100</v>
+      <c r="K46" s="30" t="s">
+        <v>103</v>
       </c>
       <c r="L46" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="M46" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="M46" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N46" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O46" s="29"/>
-      <c r="P46" s="29"/>
-      <c r="Q46" s="29"/>
-      <c r="R46" s="35"/>
-      <c r="S46" s="35"/>
+      <c r="O46" s="31"/>
+      <c r="P46" s="31"/>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="37"/>
+      <c r="S46" s="37"/>
     </row>
     <row r="47" s="1" customFormat="1" ht="45" spans="1:19">
       <c r="A47" s="21"/>
@@ -3462,7 +3480,7 @@
       <c r="D47" s="21"/>
       <c r="E47" s="11"/>
       <c r="F47" s="21" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="16" t="s">
@@ -3472,978 +3490,1019 @@
         <v>53</v>
       </c>
       <c r="J47" s="12"/>
-      <c r="K47" s="28" t="s">
-        <v>100</v>
+      <c r="K47" s="30" t="s">
+        <v>103</v>
       </c>
       <c r="L47" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="M47" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="M47" s="30" t="s">
         <v>28</v>
       </c>
       <c r="N47" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O47" s="29"/>
-      <c r="P47" s="29"/>
-      <c r="Q47" s="29"/>
-      <c r="R47" s="35"/>
-      <c r="S47" s="35"/>
-    </row>
-    <row r="48" s="2" customFormat="1" ht="45" spans="1:28">
-      <c r="A48" s="23"/>
-      <c r="B48" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
-      <c r="M48" s="25"/>
-      <c r="N48" s="30"/>
-      <c r="O48" s="23"/>
-      <c r="P48" s="23"/>
-      <c r="Q48" s="23"/>
-      <c r="R48" s="23"/>
-      <c r="S48" s="23"/>
-      <c r="T48" s="23"/>
-      <c r="U48" s="36"/>
-      <c r="V48" s="36"/>
-      <c r="W48" s="36"/>
-      <c r="X48" s="36"/>
-      <c r="Y48" s="36"/>
-      <c r="Z48" s="36"/>
-      <c r="AA48" s="36"/>
-      <c r="AB48" s="36"/>
-    </row>
-    <row r="49" s="2" customFormat="1" ht="90" spans="1:28">
-      <c r="A49" s="23"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24" t="s">
+      <c r="O47" s="31"/>
+      <c r="P47" s="31"/>
+      <c r="Q47" s="31"/>
+      <c r="R47" s="37"/>
+      <c r="S47" s="37"/>
+    </row>
+    <row r="48" s="1" customFormat="1" ht="45" spans="1:19">
+      <c r="A48" s="21"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="25"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="25"/>
-      <c r="N49" s="30"/>
-      <c r="O49" s="23"/>
-      <c r="P49" s="23"/>
-      <c r="Q49" s="23"/>
-      <c r="R49" s="23"/>
-      <c r="S49" s="23"/>
-      <c r="T49" s="23"/>
-      <c r="U49" s="36"/>
-      <c r="V49" s="36"/>
-      <c r="W49" s="36"/>
-      <c r="X49" s="36"/>
-      <c r="Y49" s="36"/>
-      <c r="Z49" s="36"/>
-      <c r="AA49" s="36"/>
-      <c r="AB49" s="36"/>
-    </row>
-    <row r="50" s="2" customFormat="1" ht="45" spans="1:28">
-      <c r="A50" s="26"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="27"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I48" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="J48" s="12"/>
+      <c r="K48" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="L48" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="M48" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N48" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="O48" s="31"/>
+      <c r="P48" s="31"/>
+      <c r="Q48" s="31"/>
+      <c r="R48" s="37"/>
+      <c r="S48" s="37"/>
+    </row>
+    <row r="49" s="2" customFormat="1" ht="45" spans="1:28">
+      <c r="A49" s="25"/>
+      <c r="B49" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="27"/>
+      <c r="L49" s="27"/>
+      <c r="M49" s="27"/>
+      <c r="N49" s="32"/>
+      <c r="O49" s="25"/>
+      <c r="P49" s="25"/>
+      <c r="Q49" s="25"/>
+      <c r="R49" s="25"/>
+      <c r="S49" s="25"/>
+      <c r="T49" s="25"/>
+      <c r="U49" s="38"/>
+      <c r="V49" s="38"/>
+      <c r="W49" s="38"/>
+      <c r="X49" s="38"/>
+      <c r="Y49" s="38"/>
+      <c r="Z49" s="38"/>
+      <c r="AA49" s="38"/>
+      <c r="AB49" s="38"/>
+    </row>
+    <row r="50" s="2" customFormat="1" ht="90" spans="1:28">
+      <c r="A50" s="25"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26" t="s">
+        <v>124</v>
+      </c>
       <c r="D50" s="26"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="G50" s="28"/>
-      <c r="H50" s="28" t="s">
+      <c r="E50" s="26"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="27"/>
+      <c r="L50" s="27"/>
+      <c r="M50" s="27"/>
+      <c r="N50" s="32"/>
+      <c r="O50" s="25"/>
+      <c r="P50" s="25"/>
+      <c r="Q50" s="25"/>
+      <c r="R50" s="25"/>
+      <c r="S50" s="25"/>
+      <c r="T50" s="25"/>
+      <c r="U50" s="38"/>
+      <c r="V50" s="38"/>
+      <c r="W50" s="38"/>
+      <c r="X50" s="38"/>
+      <c r="Y50" s="38"/>
+      <c r="Z50" s="38"/>
+      <c r="AA50" s="38"/>
+      <c r="AB50" s="38"/>
+    </row>
+    <row r="51" s="2" customFormat="1" ht="45" spans="1:28">
+      <c r="A51" s="28"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I50" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="J50" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="K50" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="L50" s="28" t="s">
+      <c r="I51" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="M50" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N50" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="O50" s="26"/>
-      <c r="P50" s="26"/>
-      <c r="Q50" s="26"/>
-      <c r="R50" s="26"/>
-      <c r="S50" s="26"/>
-      <c r="T50" s="26"/>
-      <c r="U50" s="36"/>
-      <c r="V50" s="36"/>
-      <c r="W50" s="36"/>
-      <c r="X50" s="36"/>
-      <c r="Y50" s="36"/>
-      <c r="Z50" s="36"/>
-      <c r="AA50" s="36"/>
-      <c r="AB50" s="36"/>
-    </row>
-    <row r="51" s="2" customFormat="1" ht="45" spans="1:28">
-      <c r="A51" s="26"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="28" t="s">
+      <c r="J51" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="G51" s="28"/>
-      <c r="H51" s="28" t="s">
+      <c r="K51" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="L51" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="M51" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N51" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="O51" s="28"/>
+      <c r="P51" s="28"/>
+      <c r="Q51" s="28"/>
+      <c r="R51" s="28"/>
+      <c r="S51" s="28"/>
+      <c r="T51" s="28"/>
+      <c r="U51" s="38"/>
+      <c r="V51" s="38"/>
+      <c r="W51" s="38"/>
+      <c r="X51" s="38"/>
+      <c r="Y51" s="38"/>
+      <c r="Z51" s="38"/>
+      <c r="AA51" s="38"/>
+      <c r="AB51" s="38"/>
+    </row>
+    <row r="52" s="2" customFormat="1" ht="45" spans="1:28">
+      <c r="A52" s="28"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="G52" s="30"/>
+      <c r="H52" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I51" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="J51" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="K51" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="L51" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="M51" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N51" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="O51" s="26"/>
-      <c r="P51" s="26"/>
-      <c r="Q51" s="26"/>
-      <c r="R51" s="26"/>
-      <c r="S51" s="26"/>
-      <c r="T51" s="26"/>
-      <c r="U51" s="36"/>
-      <c r="V51" s="36"/>
-      <c r="W51" s="36"/>
-      <c r="X51" s="36"/>
-      <c r="Y51" s="36"/>
-      <c r="Z51" s="36"/>
-      <c r="AA51" s="36"/>
-      <c r="AB51" s="36"/>
-    </row>
-    <row r="52" s="2" customFormat="1" ht="75" spans="1:28">
-      <c r="A52" s="26"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="28" t="s">
+      <c r="I52" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="J52" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="G52" s="28"/>
-      <c r="H52" s="28" t="s">
+      <c r="K52" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="L52" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="M52" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N52" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="O52" s="28"/>
+      <c r="P52" s="28"/>
+      <c r="Q52" s="28"/>
+      <c r="R52" s="28"/>
+      <c r="S52" s="28"/>
+      <c r="T52" s="28"/>
+      <c r="U52" s="38"/>
+      <c r="V52" s="38"/>
+      <c r="W52" s="38"/>
+      <c r="X52" s="38"/>
+      <c r="Y52" s="38"/>
+      <c r="Z52" s="38"/>
+      <c r="AA52" s="38"/>
+      <c r="AB52" s="38"/>
+    </row>
+    <row r="53" s="2" customFormat="1" ht="75" spans="1:28">
+      <c r="A53" s="28"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G53" s="30"/>
+      <c r="H53" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I52" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="J52" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="K52" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="L52" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="M52" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N52" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="O52" s="26"/>
-      <c r="P52" s="26"/>
-      <c r="Q52" s="26"/>
-      <c r="R52" s="26"/>
-      <c r="S52" s="26"/>
-      <c r="T52" s="26"/>
-      <c r="U52" s="36"/>
-      <c r="V52" s="36"/>
-      <c r="W52" s="36"/>
-      <c r="X52" s="36"/>
-      <c r="Y52" s="36"/>
-      <c r="Z52" s="36"/>
-      <c r="AA52" s="36"/>
-      <c r="AB52" s="36"/>
-    </row>
-    <row r="53" s="2" customFormat="1" ht="45" spans="1:28">
-      <c r="A53" s="26"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="28" t="s">
+      <c r="I53" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="J53" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="G53" s="28"/>
-      <c r="H53" s="28" t="s">
+      <c r="K53" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="L53" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="M53" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N53" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="O53" s="28"/>
+      <c r="P53" s="28"/>
+      <c r="Q53" s="28"/>
+      <c r="R53" s="28"/>
+      <c r="S53" s="28"/>
+      <c r="T53" s="28"/>
+      <c r="U53" s="38"/>
+      <c r="V53" s="38"/>
+      <c r="W53" s="38"/>
+      <c r="X53" s="38"/>
+      <c r="Y53" s="38"/>
+      <c r="Z53" s="38"/>
+      <c r="AA53" s="38"/>
+      <c r="AB53" s="38"/>
+    </row>
+    <row r="54" s="2" customFormat="1" ht="45" spans="1:28">
+      <c r="A54" s="28"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="G54" s="30"/>
+      <c r="H54" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I53" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="J53" s="28"/>
-      <c r="K53" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="L53" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="M53" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N53" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="O53" s="26"/>
-      <c r="P53" s="26"/>
-      <c r="Q53" s="26"/>
-      <c r="R53" s="26"/>
-      <c r="S53" s="26"/>
-      <c r="T53" s="26"/>
-      <c r="U53" s="36"/>
-      <c r="V53" s="36"/>
-      <c r="W53" s="36"/>
-      <c r="X53" s="36"/>
-      <c r="Y53" s="36"/>
-      <c r="Z53" s="36"/>
-      <c r="AA53" s="36"/>
-      <c r="AB53" s="36"/>
-    </row>
-    <row r="54" s="2" customFormat="1" ht="30" spans="1:28">
-      <c r="A54" s="23"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24" t="s">
-        <v>138</v>
-      </c>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
-      <c r="L54" s="25"/>
-      <c r="M54" s="25"/>
-      <c r="N54" s="30"/>
-      <c r="O54" s="23"/>
-      <c r="P54" s="23"/>
-      <c r="Q54" s="23"/>
-      <c r="R54" s="23"/>
-      <c r="S54" s="23"/>
-      <c r="T54" s="23"/>
-      <c r="U54" s="36"/>
-      <c r="V54" s="36"/>
-      <c r="W54" s="36"/>
-      <c r="X54" s="36"/>
-      <c r="Y54" s="36"/>
-      <c r="Z54" s="36"/>
-      <c r="AA54" s="36"/>
-      <c r="AB54" s="36"/>
+      <c r="I54" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="J54" s="30"/>
+      <c r="K54" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="L54" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="M54" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N54" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="O54" s="28"/>
+      <c r="P54" s="28"/>
+      <c r="Q54" s="28"/>
+      <c r="R54" s="28"/>
+      <c r="S54" s="28"/>
+      <c r="T54" s="28"/>
+      <c r="U54" s="38"/>
+      <c r="V54" s="38"/>
+      <c r="W54" s="38"/>
+      <c r="X54" s="38"/>
+      <c r="Y54" s="38"/>
+      <c r="Z54" s="38"/>
+      <c r="AA54" s="38"/>
+      <c r="AB54" s="38"/>
     </row>
     <row r="55" s="2" customFormat="1" ht="30" spans="1:28">
-      <c r="A55" s="26"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26" t="s">
+        <v>141</v>
+      </c>
       <c r="D55" s="26"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="G55" s="28"/>
-      <c r="H55" s="28" t="s">
+      <c r="E55" s="26"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="27"/>
+      <c r="J55" s="27"/>
+      <c r="K55" s="27"/>
+      <c r="L55" s="27"/>
+      <c r="M55" s="27"/>
+      <c r="N55" s="32"/>
+      <c r="O55" s="25"/>
+      <c r="P55" s="25"/>
+      <c r="Q55" s="25"/>
+      <c r="R55" s="25"/>
+      <c r="S55" s="25"/>
+      <c r="T55" s="25"/>
+      <c r="U55" s="38"/>
+      <c r="V55" s="38"/>
+      <c r="W55" s="38"/>
+      <c r="X55" s="38"/>
+      <c r="Y55" s="38"/>
+      <c r="Z55" s="38"/>
+      <c r="AA55" s="38"/>
+      <c r="AB55" s="38"/>
+    </row>
+    <row r="56" s="2" customFormat="1" ht="30" spans="1:28">
+      <c r="A56" s="28"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="G56" s="30"/>
+      <c r="H56" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I55" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="J55" s="28"/>
-      <c r="K55" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="L55" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="M55" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N55" s="31"/>
-      <c r="O55" s="26"/>
-      <c r="P55" s="26"/>
-      <c r="Q55" s="26"/>
-      <c r="R55" s="26"/>
-      <c r="S55" s="26"/>
-      <c r="T55" s="26"/>
-      <c r="U55" s="36"/>
-      <c r="V55" s="36"/>
-      <c r="W55" s="36"/>
-      <c r="X55" s="36"/>
-      <c r="Y55" s="36"/>
-      <c r="Z55" s="36"/>
-      <c r="AA55" s="36"/>
-      <c r="AB55" s="36"/>
-    </row>
-    <row r="56" s="2" customFormat="1" ht="75" spans="1:28">
-      <c r="A56" s="26"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="28" t="s">
+      <c r="I56" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="G56" s="28"/>
-      <c r="H56" s="28" t="s">
+      <c r="J56" s="30"/>
+      <c r="K56" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="L56" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="M56" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N56" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="O56" s="28"/>
+      <c r="P56" s="28"/>
+      <c r="Q56" s="28"/>
+      <c r="R56" s="28"/>
+      <c r="S56" s="28"/>
+      <c r="T56" s="28"/>
+      <c r="U56" s="38"/>
+      <c r="V56" s="38"/>
+      <c r="W56" s="38"/>
+      <c r="X56" s="38"/>
+      <c r="Y56" s="38"/>
+      <c r="Z56" s="38"/>
+      <c r="AA56" s="38"/>
+      <c r="AB56" s="38"/>
+    </row>
+    <row r="57" s="2" customFormat="1" ht="75" spans="1:28">
+      <c r="A57" s="28"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="G57" s="30"/>
+      <c r="H57" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I56" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="J56" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="K56" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="L56" s="28" t="s">
+      <c r="I57" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="J57" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="K57" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="L57" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="M57" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N57" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="O57" s="28"/>
+      <c r="P57" s="28"/>
+      <c r="Q57" s="28"/>
+      <c r="R57" s="28"/>
+      <c r="S57" s="28"/>
+      <c r="T57" s="28"/>
+      <c r="U57" s="38"/>
+      <c r="V57" s="38"/>
+      <c r="W57" s="38"/>
+      <c r="X57" s="38"/>
+      <c r="Y57" s="38"/>
+      <c r="Z57" s="38"/>
+      <c r="AA57" s="38"/>
+      <c r="AB57" s="38"/>
+    </row>
+    <row r="58" s="2" customFormat="1" ht="75" spans="1:28">
+      <c r="A58" s="28"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G58" s="30"/>
+      <c r="H58" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="I58" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="J58" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="K58" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="L58" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="M58" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N58" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="O58" s="28"/>
+      <c r="P58" s="28"/>
+      <c r="Q58" s="28"/>
+      <c r="R58" s="28"/>
+      <c r="S58" s="28"/>
+      <c r="T58" s="28"/>
+      <c r="U58" s="38"/>
+      <c r="V58" s="38"/>
+      <c r="W58" s="38"/>
+      <c r="X58" s="38"/>
+      <c r="Y58" s="38"/>
+      <c r="Z58" s="38"/>
+      <c r="AA58" s="38"/>
+      <c r="AB58" s="38"/>
+    </row>
+    <row r="59" s="2" customFormat="1" ht="75" spans="1:28">
+      <c r="A59" s="28"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="G59" s="30"/>
+      <c r="H59" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="I59" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="J59" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="K59" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="L59" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="M59" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N59" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="O59" s="28"/>
+      <c r="P59" s="28"/>
+      <c r="Q59" s="28"/>
+      <c r="R59" s="28"/>
+      <c r="S59" s="28"/>
+      <c r="T59" s="28"/>
+      <c r="U59" s="38"/>
+      <c r="V59" s="38"/>
+      <c r="W59" s="38"/>
+      <c r="X59" s="38"/>
+      <c r="Y59" s="38"/>
+      <c r="Z59" s="38"/>
+      <c r="AA59" s="38"/>
+      <c r="AB59" s="38"/>
+    </row>
+    <row r="60" s="2" customFormat="1" ht="30" spans="1:28">
+      <c r="A60" s="28"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="G60" s="30"/>
+      <c r="H60" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I60" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="J60" s="30"/>
+      <c r="K60" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="L60" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="M60" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N60" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="O60" s="28"/>
+      <c r="P60" s="28"/>
+      <c r="Q60" s="28"/>
+      <c r="R60" s="28"/>
+      <c r="S60" s="28"/>
+      <c r="T60" s="28"/>
+      <c r="U60" s="38"/>
+      <c r="V60" s="38"/>
+      <c r="W60" s="38"/>
+      <c r="X60" s="38"/>
+      <c r="Y60" s="38"/>
+      <c r="Z60" s="38"/>
+      <c r="AA60" s="38"/>
+      <c r="AB60" s="38"/>
+    </row>
+    <row r="61" s="2" customFormat="1" ht="15.6" spans="1:28">
+      <c r="A61" s="25"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="27"/>
+      <c r="I61" s="27"/>
+      <c r="J61" s="27"/>
+      <c r="K61" s="27"/>
+      <c r="L61" s="27"/>
+      <c r="M61" s="27"/>
+      <c r="N61" s="32"/>
+      <c r="O61" s="25"/>
+      <c r="P61" s="25"/>
+      <c r="Q61" s="25"/>
+      <c r="R61" s="25"/>
+      <c r="S61" s="25"/>
+      <c r="T61" s="25"/>
+      <c r="U61" s="38"/>
+      <c r="V61" s="38"/>
+      <c r="W61" s="38"/>
+      <c r="X61" s="38"/>
+      <c r="Y61" s="38"/>
+      <c r="Z61" s="38"/>
+      <c r="AA61" s="38"/>
+      <c r="AB61" s="38"/>
+    </row>
+    <row r="62" s="2" customFormat="1" ht="45" spans="1:28">
+      <c r="A62" s="28"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="29"/>
+      <c r="F62" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="M56" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N56" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="O56" s="26"/>
-      <c r="P56" s="26"/>
-      <c r="Q56" s="26"/>
-      <c r="R56" s="26"/>
-      <c r="S56" s="26"/>
-      <c r="T56" s="26"/>
-      <c r="U56" s="36"/>
-      <c r="V56" s="36"/>
-      <c r="W56" s="36"/>
-      <c r="X56" s="36"/>
-      <c r="Y56" s="36"/>
-      <c r="Z56" s="36"/>
-      <c r="AA56" s="36"/>
-      <c r="AB56" s="36"/>
-    </row>
-    <row r="57" s="2" customFormat="1" ht="75" spans="1:28">
-      <c r="A57" s="26"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="28" t="s">
+      <c r="G62" s="30"/>
+      <c r="H62" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I62" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="J62" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="G57" s="28"/>
-      <c r="H57" s="28" t="s">
+      <c r="K62" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="L62" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="M62" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N62" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="O62" s="28"/>
+      <c r="P62" s="28"/>
+      <c r="Q62" s="28"/>
+      <c r="R62" s="28"/>
+      <c r="S62" s="28"/>
+      <c r="T62" s="28"/>
+      <c r="U62" s="38"/>
+      <c r="V62" s="38"/>
+      <c r="W62" s="38"/>
+      <c r="X62" s="38"/>
+      <c r="Y62" s="38"/>
+      <c r="Z62" s="38"/>
+      <c r="AA62" s="38"/>
+      <c r="AB62" s="38"/>
+    </row>
+    <row r="63" s="2" customFormat="1" ht="45" spans="1:28">
+      <c r="A63" s="28"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G63" s="30"/>
+      <c r="H63" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="I57" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="J57" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="K57" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="L57" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="M57" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N57" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="O57" s="26"/>
-      <c r="P57" s="26"/>
-      <c r="Q57" s="26"/>
-      <c r="R57" s="26"/>
-      <c r="S57" s="26"/>
-      <c r="T57" s="26"/>
-      <c r="U57" s="36"/>
-      <c r="V57" s="36"/>
-      <c r="W57" s="36"/>
-      <c r="X57" s="36"/>
-      <c r="Y57" s="36"/>
-      <c r="Z57" s="36"/>
-      <c r="AA57" s="36"/>
-      <c r="AB57" s="36"/>
-    </row>
-    <row r="58" s="2" customFormat="1" ht="75" spans="1:28">
-      <c r="A58" s="26"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="G58" s="28"/>
-      <c r="H58" s="28" t="s">
+      <c r="I63" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="J63" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="K63" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="L63" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="M63" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N63" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="O63" s="28"/>
+      <c r="P63" s="28"/>
+      <c r="Q63" s="28"/>
+      <c r="R63" s="28"/>
+      <c r="S63" s="28"/>
+      <c r="T63" s="28"/>
+      <c r="U63" s="38"/>
+      <c r="V63" s="38"/>
+      <c r="W63" s="38"/>
+      <c r="X63" s="38"/>
+      <c r="Y63" s="38"/>
+      <c r="Z63" s="38"/>
+      <c r="AA63" s="38"/>
+      <c r="AB63" s="38"/>
+    </row>
+    <row r="64" s="2" customFormat="1" ht="45" spans="1:28">
+      <c r="A64" s="28"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="G64" s="30"/>
+      <c r="H64" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="I58" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="J58" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="K58" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="L58" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="M58" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N58" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="O58" s="26"/>
-      <c r="P58" s="26"/>
-      <c r="Q58" s="26"/>
-      <c r="R58" s="26"/>
-      <c r="S58" s="26"/>
-      <c r="T58" s="26"/>
-      <c r="U58" s="36"/>
-      <c r="V58" s="36"/>
-      <c r="W58" s="36"/>
-      <c r="X58" s="36"/>
-      <c r="Y58" s="36"/>
-      <c r="Z58" s="36"/>
-      <c r="AA58" s="36"/>
-      <c r="AB58" s="36"/>
-    </row>
-    <row r="59" s="2" customFormat="1" ht="30" spans="1:28">
-      <c r="A59" s="26"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="28" t="s">
+      <c r="I64" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="J64" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="G59" s="28"/>
-      <c r="H59" s="28" t="s">
+      <c r="K64" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="L64" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="M64" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N64" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="O64" s="28"/>
+      <c r="P64" s="28"/>
+      <c r="Q64" s="28"/>
+      <c r="R64" s="28"/>
+      <c r="S64" s="28"/>
+      <c r="T64" s="28"/>
+      <c r="U64" s="38"/>
+      <c r="V64" s="38"/>
+      <c r="W64" s="38"/>
+      <c r="X64" s="38"/>
+      <c r="Y64" s="38"/>
+      <c r="Z64" s="38"/>
+      <c r="AA64" s="38"/>
+      <c r="AB64" s="38"/>
+    </row>
+    <row r="65" s="2" customFormat="1" ht="30" spans="1:28">
+      <c r="A65" s="25"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="27"/>
+      <c r="H65" s="27"/>
+      <c r="I65" s="27"/>
+      <c r="J65" s="27"/>
+      <c r="K65" s="27"/>
+      <c r="L65" s="27"/>
+      <c r="M65" s="27"/>
+      <c r="N65" s="32"/>
+      <c r="O65" s="25"/>
+      <c r="P65" s="25"/>
+      <c r="Q65" s="25"/>
+      <c r="R65" s="25"/>
+      <c r="S65" s="25"/>
+      <c r="T65" s="25"/>
+      <c r="U65" s="38"/>
+      <c r="V65" s="38"/>
+      <c r="W65" s="38"/>
+      <c r="X65" s="38"/>
+      <c r="Y65" s="38"/>
+      <c r="Z65" s="38"/>
+      <c r="AA65" s="38"/>
+      <c r="AB65" s="38"/>
+    </row>
+    <row r="66" s="2" customFormat="1" ht="45" spans="1:28">
+      <c r="A66" s="28"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="G66" s="30"/>
+      <c r="H66" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I59" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="J59" s="28"/>
-      <c r="K59" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="L59" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="M59" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N59" s="31"/>
-      <c r="O59" s="26"/>
-      <c r="P59" s="26"/>
-      <c r="Q59" s="26"/>
-      <c r="R59" s="26"/>
-      <c r="S59" s="26"/>
-      <c r="T59" s="26"/>
-      <c r="U59" s="36"/>
-      <c r="V59" s="36"/>
-      <c r="W59" s="36"/>
-      <c r="X59" s="36"/>
-      <c r="Y59" s="36"/>
-      <c r="Z59" s="36"/>
-      <c r="AA59" s="36"/>
-      <c r="AB59" s="36"/>
-    </row>
-    <row r="60" s="2" customFormat="1" ht="15.6" spans="1:28">
-      <c r="A60" s="23"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
-      <c r="I60" s="25"/>
-      <c r="J60" s="25"/>
-      <c r="K60" s="25"/>
-      <c r="L60" s="25"/>
-      <c r="M60" s="25"/>
-      <c r="N60" s="30"/>
-      <c r="O60" s="23"/>
-      <c r="P60" s="23"/>
-      <c r="Q60" s="23"/>
-      <c r="R60" s="23"/>
-      <c r="S60" s="23"/>
-      <c r="T60" s="23"/>
-      <c r="U60" s="36"/>
-      <c r="V60" s="36"/>
-      <c r="W60" s="36"/>
-      <c r="X60" s="36"/>
-      <c r="Y60" s="36"/>
-      <c r="Z60" s="36"/>
-      <c r="AA60" s="36"/>
-      <c r="AB60" s="36"/>
-    </row>
-    <row r="61" s="2" customFormat="1" ht="45" spans="1:28">
-      <c r="A61" s="26"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="27"/>
-      <c r="F61" s="28" t="s">
+      <c r="I66" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="J66" s="30"/>
+      <c r="K66" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="L66" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="M66" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N66" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="O66" s="28"/>
+      <c r="P66" s="28"/>
+      <c r="Q66" s="28"/>
+      <c r="R66" s="28"/>
+      <c r="S66" s="28"/>
+      <c r="T66" s="28"/>
+      <c r="U66" s="38"/>
+      <c r="V66" s="38"/>
+      <c r="W66" s="38"/>
+      <c r="X66" s="38"/>
+      <c r="Y66" s="38"/>
+      <c r="Z66" s="38"/>
+      <c r="AA66" s="38"/>
+      <c r="AB66" s="38"/>
+    </row>
+    <row r="67" s="2" customFormat="1" ht="45" spans="1:28">
+      <c r="A67" s="28"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="G67" s="30"/>
+      <c r="H67" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I67" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="J67" s="30"/>
+      <c r="K67" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="L67" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="M67" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N67" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="O67" s="28"/>
+      <c r="P67" s="28"/>
+      <c r="Q67" s="28"/>
+      <c r="R67" s="28"/>
+      <c r="S67" s="28"/>
+      <c r="T67" s="28"/>
+      <c r="U67" s="38"/>
+      <c r="V67" s="38"/>
+      <c r="W67" s="38"/>
+      <c r="X67" s="38"/>
+      <c r="Y67" s="38"/>
+      <c r="Z67" s="38"/>
+      <c r="AA67" s="38"/>
+      <c r="AB67" s="38"/>
+    </row>
+    <row r="68" s="2" customFormat="1" ht="60" spans="1:28">
+      <c r="A68" s="28"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="G68" s="30"/>
+      <c r="H68" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I68" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="G61" s="28"/>
-      <c r="H61" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="I61" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="J61" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="K61" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="L61" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="M61" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N61" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="O61" s="26"/>
-      <c r="P61" s="26"/>
-      <c r="Q61" s="26"/>
-      <c r="R61" s="26"/>
-      <c r="S61" s="26"/>
-      <c r="T61" s="26"/>
-      <c r="U61" s="36"/>
-      <c r="V61" s="36"/>
-      <c r="W61" s="36"/>
-      <c r="X61" s="36"/>
-      <c r="Y61" s="36"/>
-      <c r="Z61" s="36"/>
-      <c r="AA61" s="36"/>
-      <c r="AB61" s="36"/>
-    </row>
-    <row r="62" s="2" customFormat="1" ht="45" spans="1:28">
-      <c r="A62" s="26"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="G62" s="28"/>
-      <c r="H62" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="I62" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="J62" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="K62" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="L62" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="M62" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N62" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="O62" s="26"/>
-      <c r="P62" s="26"/>
-      <c r="Q62" s="26"/>
-      <c r="R62" s="26"/>
-      <c r="S62" s="26"/>
-      <c r="T62" s="26"/>
-      <c r="U62" s="36"/>
-      <c r="V62" s="36"/>
-      <c r="W62" s="36"/>
-      <c r="X62" s="36"/>
-      <c r="Y62" s="36"/>
-      <c r="Z62" s="36"/>
-      <c r="AA62" s="36"/>
-      <c r="AB62" s="36"/>
-    </row>
-    <row r="63" s="2" customFormat="1" ht="45" spans="1:28">
-      <c r="A63" s="26"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="27"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="G63" s="28"/>
-      <c r="H63" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="I63" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="J63" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="K63" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="L63" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="M63" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N63" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="O63" s="26"/>
-      <c r="P63" s="26"/>
-      <c r="Q63" s="26"/>
-      <c r="R63" s="26"/>
-      <c r="S63" s="26"/>
-      <c r="T63" s="26"/>
-      <c r="U63" s="36"/>
-      <c r="V63" s="36"/>
-      <c r="W63" s="36"/>
-      <c r="X63" s="36"/>
-      <c r="Y63" s="36"/>
-      <c r="Z63" s="36"/>
-      <c r="AA63" s="36"/>
-      <c r="AB63" s="36"/>
-    </row>
-    <row r="64" s="2" customFormat="1" ht="30" spans="1:28">
-      <c r="A64" s="23"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="25"/>
-      <c r="I64" s="25"/>
-      <c r="J64" s="25"/>
-      <c r="K64" s="25"/>
-      <c r="L64" s="25"/>
-      <c r="M64" s="25"/>
-      <c r="N64" s="30"/>
-      <c r="O64" s="23"/>
-      <c r="P64" s="23"/>
-      <c r="Q64" s="23"/>
-      <c r="R64" s="23"/>
-      <c r="S64" s="23"/>
-      <c r="T64" s="23"/>
-      <c r="U64" s="36"/>
-      <c r="V64" s="36"/>
-      <c r="W64" s="36"/>
-      <c r="X64" s="36"/>
-      <c r="Y64" s="36"/>
-      <c r="Z64" s="36"/>
-      <c r="AA64" s="36"/>
-      <c r="AB64" s="36"/>
-    </row>
-    <row r="65" s="2" customFormat="1" ht="45" spans="1:28">
-      <c r="A65" s="26"/>
-      <c r="B65" s="27"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="26"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="G65" s="28"/>
-      <c r="H65" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="I65" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="J65" s="28"/>
-      <c r="K65" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="L65" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="M65" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N65" s="31"/>
-      <c r="O65" s="26"/>
-      <c r="P65" s="26"/>
-      <c r="Q65" s="26"/>
-      <c r="R65" s="26"/>
-      <c r="S65" s="26"/>
-      <c r="T65" s="26"/>
-      <c r="U65" s="36"/>
-      <c r="V65" s="36"/>
-      <c r="W65" s="36"/>
-      <c r="X65" s="36"/>
-      <c r="Y65" s="36"/>
-      <c r="Z65" s="36"/>
-      <c r="AA65" s="36"/>
-      <c r="AB65" s="36"/>
-    </row>
-    <row r="66" s="2" customFormat="1" ht="45" spans="1:28">
-      <c r="A66" s="26"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="27"/>
-      <c r="D66" s="26"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="G66" s="28"/>
-      <c r="H66" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="I66" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="J66" s="28"/>
-      <c r="K66" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="L66" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="M66" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N66" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="O66" s="26"/>
-      <c r="P66" s="26"/>
-      <c r="Q66" s="26"/>
-      <c r="R66" s="26"/>
-      <c r="S66" s="26"/>
-      <c r="T66" s="26"/>
-      <c r="U66" s="36"/>
-      <c r="V66" s="36"/>
-      <c r="W66" s="36"/>
-      <c r="X66" s="36"/>
-      <c r="Y66" s="36"/>
-      <c r="Z66" s="36"/>
-      <c r="AA66" s="36"/>
-      <c r="AB66" s="36"/>
-    </row>
-    <row r="67" s="2" customFormat="1" ht="60" spans="1:28">
-      <c r="A67" s="26"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="26"/>
-      <c r="E67" s="27"/>
-      <c r="F67" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="G67" s="28"/>
-      <c r="H67" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="I67" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="J67" s="28"/>
-      <c r="K67" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="L67" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="M67" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N67" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="O67" s="26"/>
-      <c r="P67" s="26"/>
-      <c r="Q67" s="26"/>
-      <c r="R67" s="26"/>
-      <c r="S67" s="26"/>
-      <c r="T67" s="26"/>
-      <c r="U67" s="36"/>
-      <c r="V67" s="36"/>
-      <c r="W67" s="36"/>
-      <c r="X67" s="36"/>
-      <c r="Y67" s="36"/>
-      <c r="Z67" s="36"/>
-      <c r="AA67" s="36"/>
-      <c r="AB67" s="36"/>
-    </row>
-    <row r="68" s="2" customFormat="1" ht="15.6" spans="1:28">
-      <c r="A68" s="26"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="26"/>
-      <c r="E68" s="27"/>
-      <c r="F68" s="28"/>
-      <c r="G68" s="28"/>
-      <c r="H68" s="28"/>
-      <c r="I68" s="28"/>
-      <c r="J68" s="28"/>
-      <c r="K68" s="28"/>
-      <c r="L68" s="28"/>
-      <c r="M68" s="28"/>
-      <c r="N68" s="31"/>
-      <c r="O68" s="26"/>
-      <c r="P68" s="26"/>
-      <c r="Q68" s="26"/>
-      <c r="R68" s="26"/>
-      <c r="S68" s="26"/>
-      <c r="T68" s="26"/>
-      <c r="U68" s="36"/>
-      <c r="V68" s="36"/>
-      <c r="W68" s="36"/>
-      <c r="X68" s="36"/>
-      <c r="Y68" s="36"/>
-      <c r="Z68" s="36"/>
-      <c r="AA68" s="36"/>
-      <c r="AB68" s="36"/>
+      <c r="J68" s="30"/>
+      <c r="K68" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="L68" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="M68" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N68" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="O68" s="28"/>
+      <c r="P68" s="28"/>
+      <c r="Q68" s="28"/>
+      <c r="R68" s="28"/>
+      <c r="S68" s="28"/>
+      <c r="T68" s="28"/>
+      <c r="U68" s="38"/>
+      <c r="V68" s="38"/>
+      <c r="W68" s="38"/>
+      <c r="X68" s="38"/>
+      <c r="Y68" s="38"/>
+      <c r="Z68" s="38"/>
+      <c r="AA68" s="38"/>
+      <c r="AB68" s="38"/>
     </row>
     <row r="69" s="2" customFormat="1" ht="15.6" spans="1:28">
-      <c r="A69" s="26"/>
-      <c r="B69" s="27"/>
-      <c r="C69" s="27"/>
-      <c r="D69" s="26"/>
-      <c r="E69" s="27"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="28"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28"/>
-      <c r="K69" s="28"/>
-      <c r="L69" s="28"/>
-      <c r="M69" s="28"/>
-      <c r="N69" s="31"/>
-      <c r="O69" s="26"/>
-      <c r="P69" s="26"/>
-      <c r="Q69" s="26"/>
-      <c r="R69" s="26"/>
-      <c r="S69" s="26"/>
-      <c r="T69" s="26"/>
-      <c r="U69" s="36"/>
-      <c r="V69" s="36"/>
-      <c r="W69" s="36"/>
-      <c r="X69" s="36"/>
-      <c r="Y69" s="36"/>
-      <c r="Z69" s="36"/>
-      <c r="AA69" s="36"/>
-      <c r="AB69" s="36"/>
+      <c r="A69" s="28"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="30"/>
+      <c r="G69" s="30"/>
+      <c r="H69" s="30"/>
+      <c r="I69" s="30"/>
+      <c r="J69" s="30"/>
+      <c r="K69" s="30"/>
+      <c r="L69" s="30"/>
+      <c r="M69" s="30"/>
+      <c r="N69" s="33"/>
+      <c r="O69" s="28"/>
+      <c r="P69" s="28"/>
+      <c r="Q69" s="28"/>
+      <c r="R69" s="28"/>
+      <c r="S69" s="28"/>
+      <c r="T69" s="28"/>
+      <c r="U69" s="38"/>
+      <c r="V69" s="38"/>
+      <c r="W69" s="38"/>
+      <c r="X69" s="38"/>
+      <c r="Y69" s="38"/>
+      <c r="Z69" s="38"/>
+      <c r="AA69" s="38"/>
+      <c r="AB69" s="38"/>
     </row>
     <row r="70" s="2" customFormat="1" ht="15.6" spans="1:28">
-      <c r="A70" s="26"/>
-      <c r="B70" s="27"/>
-      <c r="C70" s="27"/>
-      <c r="D70" s="26"/>
-      <c r="E70" s="27"/>
-      <c r="F70" s="28"/>
-      <c r="G70" s="28"/>
-      <c r="H70" s="28"/>
-      <c r="I70" s="28"/>
-      <c r="J70" s="28"/>
-      <c r="K70" s="28"/>
-      <c r="L70" s="28"/>
-      <c r="M70" s="28"/>
-      <c r="N70" s="31"/>
-      <c r="O70" s="26"/>
-      <c r="P70" s="26"/>
-      <c r="Q70" s="26"/>
-      <c r="R70" s="26"/>
-      <c r="S70" s="26"/>
-      <c r="T70" s="26"/>
-      <c r="U70" s="36"/>
-      <c r="V70" s="36"/>
-      <c r="W70" s="36"/>
-      <c r="X70" s="36"/>
-      <c r="Y70" s="36"/>
-      <c r="Z70" s="36"/>
-      <c r="AA70" s="36"/>
-      <c r="AB70" s="36"/>
+      <c r="A70" s="28"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="28"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="30"/>
+      <c r="G70" s="30"/>
+      <c r="H70" s="30"/>
+      <c r="I70" s="30"/>
+      <c r="J70" s="30"/>
+      <c r="K70" s="30"/>
+      <c r="L70" s="30"/>
+      <c r="M70" s="30"/>
+      <c r="N70" s="33"/>
+      <c r="O70" s="28"/>
+      <c r="P70" s="28"/>
+      <c r="Q70" s="28"/>
+      <c r="R70" s="28"/>
+      <c r="S70" s="28"/>
+      <c r="T70" s="28"/>
+      <c r="U70" s="38"/>
+      <c r="V70" s="38"/>
+      <c r="W70" s="38"/>
+      <c r="X70" s="38"/>
+      <c r="Y70" s="38"/>
+      <c r="Z70" s="38"/>
+      <c r="AA70" s="38"/>
+      <c r="AB70" s="38"/>
     </row>
     <row r="71" s="2" customFormat="1" ht="15.6" spans="1:28">
-      <c r="A71" s="26"/>
-      <c r="B71" s="27"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="26"/>
-      <c r="E71" s="27"/>
-      <c r="F71" s="28"/>
-      <c r="G71" s="28"/>
-      <c r="H71" s="28"/>
-      <c r="I71" s="28"/>
-      <c r="J71" s="28"/>
-      <c r="K71" s="28"/>
-      <c r="L71" s="28"/>
-      <c r="M71" s="28"/>
-      <c r="N71" s="31"/>
-      <c r="O71" s="26"/>
-      <c r="P71" s="26"/>
-      <c r="Q71" s="26"/>
-      <c r="R71" s="26"/>
-      <c r="S71" s="26"/>
-      <c r="T71" s="26"/>
-      <c r="U71" s="36"/>
-      <c r="V71" s="36"/>
-      <c r="W71" s="36"/>
-      <c r="X71" s="36"/>
-      <c r="Y71" s="36"/>
-      <c r="Z71" s="36"/>
-      <c r="AA71" s="36"/>
-      <c r="AB71" s="36"/>
+      <c r="A71" s="28"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="29"/>
+      <c r="F71" s="30"/>
+      <c r="G71" s="30"/>
+      <c r="H71" s="30"/>
+      <c r="I71" s="30"/>
+      <c r="J71" s="30"/>
+      <c r="K71" s="30"/>
+      <c r="L71" s="30"/>
+      <c r="M71" s="30"/>
+      <c r="N71" s="33"/>
+      <c r="O71" s="28"/>
+      <c r="P71" s="28"/>
+      <c r="Q71" s="28"/>
+      <c r="R71" s="28"/>
+      <c r="S71" s="28"/>
+      <c r="T71" s="28"/>
+      <c r="U71" s="38"/>
+      <c r="V71" s="38"/>
+      <c r="W71" s="38"/>
+      <c r="X71" s="38"/>
+      <c r="Y71" s="38"/>
+      <c r="Z71" s="38"/>
+      <c r="AA71" s="38"/>
+      <c r="AB71" s="38"/>
+    </row>
+    <row r="72" s="2" customFormat="1" ht="15.6" spans="1:28">
+      <c r="A72" s="28"/>
+      <c r="B72" s="29"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="30"/>
+      <c r="G72" s="30"/>
+      <c r="H72" s="30"/>
+      <c r="I72" s="30"/>
+      <c r="J72" s="30"/>
+      <c r="K72" s="30"/>
+      <c r="L72" s="30"/>
+      <c r="M72" s="30"/>
+      <c r="N72" s="33"/>
+      <c r="O72" s="28"/>
+      <c r="P72" s="28"/>
+      <c r="Q72" s="28"/>
+      <c r="R72" s="28"/>
+      <c r="S72" s="28"/>
+      <c r="T72" s="28"/>
+      <c r="U72" s="38"/>
+      <c r="V72" s="38"/>
+      <c r="W72" s="38"/>
+      <c r="X72" s="38"/>
+      <c r="Y72" s="38"/>
+      <c r="Z72" s="38"/>
+      <c r="AA72" s="38"/>
+      <c r="AB72" s="38"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB67">
+  <autoFilter ref="A1:AB68">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>